<commit_message>
Updated Common_FP_Plots to work consistently and did line graphs.
updated summary stats output sheet name as well becasue it was truncating.
</commit_message>
<xml_diff>
--- a/Working Directory/Output/Summary_DE_Genes_by_Samples_Stats.xlsx
+++ b/Working Directory/Output/Summary_DE_Genes_by_Samples_Stats.xlsx
@@ -7,24 +7,24 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="3_500_500_outliers_upregulate" sheetId="1" r:id="rId1"/>
-    <sheet name="3_500_500_outliers_downregula" sheetId="2" r:id="rId2"/>
-    <sheet name="3_750_250_outliers_upregulate" sheetId="3" r:id="rId3"/>
-    <sheet name="3_750_250_outliers_downregula" sheetId="4" r:id="rId4"/>
-    <sheet name="3_1000_0_outliers_upregulated" sheetId="5" r:id="rId5"/>
-    <sheet name="3_1000_0_outliers_downregulat" sheetId="6" r:id="rId6"/>
-    <sheet name="6_500_500_outliers_upregulate" sheetId="7" r:id="rId7"/>
-    <sheet name="6_500_500_outliers_downregula" sheetId="8" r:id="rId8"/>
-    <sheet name="6_750_250_outliers_upregulate" sheetId="9" r:id="rId9"/>
-    <sheet name="6_750_250_outliers_downregula" sheetId="10" r:id="rId10"/>
-    <sheet name="6_1000_0_outliers_upregulated" sheetId="11" r:id="rId11"/>
-    <sheet name="6_1000_0_outliers_downregulat" sheetId="12" r:id="rId12"/>
-    <sheet name="9_500_500_outliers_upregulate" sheetId="13" r:id="rId13"/>
-    <sheet name="9_500_500_outliers_downregula" sheetId="14" r:id="rId14"/>
-    <sheet name="9_750_250_outliers_upregulate" sheetId="15" r:id="rId15"/>
-    <sheet name="9_750_250_outliers_downregula" sheetId="16" r:id="rId16"/>
-    <sheet name="9_1000_0_outliers_upregulated" sheetId="17" r:id="rId17"/>
-    <sheet name="9_1000_0_outliers_downregulat" sheetId="18" r:id="rId18"/>
+    <sheet name="3_500_500_fp_upregulated" sheetId="1" r:id="rId1"/>
+    <sheet name="3_500_500_fp_downregulated" sheetId="2" r:id="rId2"/>
+    <sheet name="3_750_250_fp_upregulated" sheetId="3" r:id="rId3"/>
+    <sheet name="3_750_250_fp_downregulated" sheetId="4" r:id="rId4"/>
+    <sheet name="3_1000_0_fp_upregulated" sheetId="5" r:id="rId5"/>
+    <sheet name="3_1000_0_fp_downregulated" sheetId="6" r:id="rId6"/>
+    <sheet name="6_500_500_fp_upregulated" sheetId="7" r:id="rId7"/>
+    <sheet name="6_500_500_fp_downregulated" sheetId="8" r:id="rId8"/>
+    <sheet name="6_750_250_fp_upregulated" sheetId="9" r:id="rId9"/>
+    <sheet name="6_750_250_fp_downregulated" sheetId="10" r:id="rId10"/>
+    <sheet name="6_1000_0_fp_upregulated" sheetId="11" r:id="rId11"/>
+    <sheet name="6_1000_0_fp_downregulated" sheetId="12" r:id="rId12"/>
+    <sheet name="9_500_500_fp_upregulated" sheetId="13" r:id="rId13"/>
+    <sheet name="9_500_500_fp_downregulated" sheetId="14" r:id="rId14"/>
+    <sheet name="9_750_250_fp_upregulated" sheetId="15" r:id="rId15"/>
+    <sheet name="9_750_250_fp_downregulated" sheetId="16" r:id="rId16"/>
+    <sheet name="9_1000_0_fp_upregulated" sheetId="17" r:id="rId17"/>
+    <sheet name="9_1000_0_fp_downregulated" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>